<commit_message>
Fix bugs: lefted suggestions, NaN%, search, footer
</commit_message>
<xml_diff>
--- a/server/routes/question-workbook.xlsx
+++ b/server/routes/question-workbook.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Тип вопроса</t>
   </si>
@@ -28,19 +28,22 @@
     <t>Количество неправильных ответов</t>
   </si>
   <si>
+    <t>one answer</t>
+  </si>
+  <si>
+    <t>да</t>
+  </si>
+  <si>
     <t>without answer option</t>
   </si>
   <si>
-    <t>да</t>
-  </si>
-  <si>
     <t>without answer with verification</t>
   </si>
   <si>
-    <t>one answer</t>
-  </si>
-  <si>
     <t>multiple answers</t>
+  </si>
+  <si>
+    <t>нет</t>
   </si>
 </sst>
 </file>
@@ -446,13 +449,10 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -460,19 +460,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
       <c r="E3">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -480,16 +477,13 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
       <c r="E4">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -497,13 +491,10 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
       </c>
       <c r="E5">
         <v>6</v>
@@ -511,16 +502,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
       </c>
       <c r="E6">
         <v>6</v>
@@ -531,13 +519,10 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
       </c>
       <c r="E7">
         <v>6</v>
@@ -548,33 +533,27 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
       <c r="E8">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
       <c r="E9">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -582,16 +561,321 @@
         <v>8</v>
       </c>
       <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10">
-        <v>6</v>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>